<commit_message>
Round1 with results for both config
</commit_message>
<xml_diff>
--- a/sanitized.xlsx
+++ b/sanitized.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27322"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="80" windowWidth="30560" windowHeight="16100"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="19440" windowHeight="12240" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="impacts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="omnetpp" sheetId="11" r:id="rId11"/>
     <sheet name="milc" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -803,17 +803,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="23"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>38</v>
       </c>
@@ -821,7 +821,7 @@
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -841,7 +841,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="29" customFormat="1">
+    <row r="3" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>19</v>
       </c>
@@ -865,7 +865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -889,7 +889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -913,7 +913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="29" customFormat="1">
+    <row r="6" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>22</v>
       </c>
@@ -937,7 +937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="25" customFormat="1">
+    <row r="7" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
@@ -961,7 +961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -985,7 +985,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="29" customFormat="1">
+    <row r="9" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>25</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="29" customFormat="1">
+    <row r="11" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>27</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="29" customFormat="1">
+    <row r="13" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>29</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="29" customFormat="1">
+    <row r="14" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>30</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="29" customFormat="1">
+    <row r="15" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>31</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="29" customFormat="1">
+    <row r="16" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>32</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="29" customFormat="1">
+    <row r="17" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>33</v>
       </c>
@@ -1219,21 +1219,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D20" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>0.42000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>0.45000000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>0.72000000000000008</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>0.76000000000000012</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>0.8600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>0.92000000000000015</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>12</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>0.96000000000000019</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18">
         <f>SUM(C3:C17)</f>
         <v>1.0000000000000002</v>
@@ -1667,10 +1667,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G19" s="22"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="G20" s="22"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -1689,12 +1689,12 @@
       </c>
       <c r="G21" s="22"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>59</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>1</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>2</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>3</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>4</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>0.79600000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>5</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>0.84600000000000009</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>6</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>0.88600000000000012</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>7</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>0.89000000000000012</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>8</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>0.91000000000000014</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>9</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>0.93000000000000016</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>10</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>0.94000000000000017</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>11</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0.9700000000000002</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>12</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>0.9800000000000002</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>13</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>0.99000000000000021</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>14</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C40">
         <f>SUM(C25:C39)</f>
         <v>1.0000000000000002</v>
@@ -2142,21 +2142,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>0.38000000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>0.43000000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>0.72000000000000008</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>0.76000000000000012</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>0.8600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>0.92000000000000015</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>12</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>0.96000000000000019</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>0.99000000000000021</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18">
         <f>SUM(C3:C17)</f>
         <v>1.0000000000000002</v>
@@ -2587,7 +2587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>59</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>1</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>2</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>3</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>0.69500000000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>4</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>0.81500000000000006</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>5</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>6</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>7</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>0.94500000000000006</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>8</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>0.95500000000000007</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>9</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0.96000000000000008</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>10</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>0.98000000000000009</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>11</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>0.9930000000000001</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>12</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>0.99800000000000011</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>13</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>0.99900000000000011</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>14</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C39">
         <f>SUM(C24:C38)</f>
         <v>1</v>
@@ -3035,7 +3035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G40" s="22" t="s">
         <v>45</v>
       </c>
@@ -3058,22 +3058,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="4"/>
-    <col min="7" max="7" width="10.83203125" style="22"/>
+    <col min="4" max="4" width="10.85546875" style="4"/>
+    <col min="7" max="7" width="10.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>0.66000000000000014</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>0.71000000000000019</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>12</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>0.76000000000000023</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>0.77000000000000024</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>0.79000000000000026</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>0.81000000000000028</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>16</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>0.82000000000000028</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>17</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>0.8400000000000003</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>18</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>0.86000000000000032</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>19</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>0.87000000000000033</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>20</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>0.88000000000000034</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>21</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>0.89000000000000035</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>22</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>0.91000000000000036</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>23</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>0.92000000000000037</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>24</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>0.93000000000000038</v>
       </c>
     </row>
-    <row r="28" spans="2:10">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>25</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>0.96000000000000041</v>
       </c>
     </row>
-    <row r="29" spans="2:10">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>26</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>0.97000000000000042</v>
       </c>
     </row>
-    <row r="30" spans="2:10">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>27</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>0.98000000000000043</v>
       </c>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>28</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>0.99000000000000044</v>
       </c>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>29</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C33">
         <f>SUM(C3:C32)</f>
         <v>1.0000000000000004</v>
@@ -3897,12 +3897,12 @@
         <v>1.0000000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>59</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>0.19400000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>1</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>0.30399999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>2</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>3</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>4</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>5</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>0.64400000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>6</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>0.69400000000000006</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>7</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>0.74400000000000011</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>8</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>0.75900000000000012</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>9</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>0.79900000000000015</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>10</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>0.81900000000000017</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>11</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>0.83900000000000019</v>
       </c>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>12</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>0.86900000000000022</v>
       </c>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>13</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>0.87900000000000023</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>14</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>0.88600000000000023</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>15</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>0.89300000000000024</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>16</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>0.90300000000000025</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>17</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>0.91500000000000026</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>18</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>0.92500000000000027</v>
       </c>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>19</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>0.93500000000000028</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>20</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>0.94200000000000028</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>21</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>0.94700000000000029</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>22</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>0.95700000000000029</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>23</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>0.9670000000000003</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>24</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>0.97000000000000031</v>
       </c>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>25</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>0.98000000000000032</v>
       </c>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>26</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>0.98500000000000032</v>
       </c>
     </row>
-    <row r="64" spans="2:9">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>27</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>0.99000000000000032</v>
       </c>
     </row>
-    <row r="65" spans="2:9">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>28</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>0.99500000000000033</v>
       </c>
     </row>
-    <row r="66" spans="2:9">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>29</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="67" spans="2:9">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C67">
         <f>SUM(C37:C66)</f>
         <v>1.0000000000000002</v>
@@ -4742,13 +4742,13 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>15</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>64203643.133333303</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>102177328.058824</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>42088905.25</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>54883486.625</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>64090230.142857097</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>65195183.625</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>46803639.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>47237670.714285702</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>50638457.714285702</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>55945417.888888903</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>81889749.535714298</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>51869571.727272697</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>88381438.066666707</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>53790349.125</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -4987,16 +4987,16 @@
       <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="7" width="16.33203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="5" max="7" width="16.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="13" customFormat="1">
+    <row r="1" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>48</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>39</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0.03</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.16</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0.09</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.12</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>0.42000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.11</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.13</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.36</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -5290,10 +5290,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="42">
+    <row r="12" spans="1:14" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>49</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.02</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>7.2319201995012475E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.2</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>0.21695760598503741</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>0.1</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>9.9750623441396506E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.1</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>3.4912718204488775E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.08</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>1.2468827930174564E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0.1</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>5.4862842892768077E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.4</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>0.59850374064837908</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D20">
         <f>SUM(D13:D19)</f>
         <v>1</v>
@@ -5668,7 +5668,7 @@
         <v>100075000</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>62</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -5704,15 +5704,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0.02</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>0.10406698564593302</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0.2</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>0.10645933014354067</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.1</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>1.076555023923445E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>0.1</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>1.7942583732057416E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0.08</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>4.7846889952153108E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.1</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>2.2727272727272728E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0.4</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>0.73325358851674638</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D34">
         <f>SUM(D27:D33)</f>
         <v>1</v>
@@ -6086,7 +6086,7 @@
         <v>104550000</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0.02</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>5.5693069306930694E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0.2</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>5.5074257425742575E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>0.1</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>6.8069306930693069E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.1</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>1.2995049504950494E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>0.08</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>1.2376237623762376E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>0.1</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>1.7326732673267328E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>0.4</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>0.8508663366336634</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D45">
         <f>SUM(D38:D44)</f>
         <v>1</v>
@@ -6460,12 +6460,12 @@
         <v>100095000</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>69</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="2:14">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>0.02</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>2.5815704553603443E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:14">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>0.2</v>
       </c>
@@ -6591,7 +6591,7 @@
         <v>0.31946934385084258</v>
       </c>
     </row>
-    <row r="51" spans="2:14">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>0.1</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>2.509860164933668E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:14">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>0.1</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>6.4539261384008607E-3</v>
       </c>
     </row>
-    <row r="53" spans="2:14">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>0.08</v>
       </c>
@@ -6723,7 +6723,7 @@
         <v>1.7569021154535677E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:14">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>0.1</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>8.8562208676945142E-2</v>
       </c>
     </row>
-    <row r="55" spans="2:14">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>0.4</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>0.51703119397633557</v>
       </c>
     </row>
-    <row r="56" spans="2:14">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D56">
         <f>SUM(D49:D55)</f>
         <v>1</v>
@@ -6855,25 +6855,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="22" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="4" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>0.12000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15">
         <f>SUM(C3:C14)</f>
         <v>1</v>
@@ -7235,7 +7235,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -7243,17 +7243,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>59</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1</v>
       </c>
@@ -7339,7 +7339,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>2</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>3</v>
       </c>
@@ -7391,7 +7391,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>4</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>5</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>6</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>7</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>8</v>
       </c>
@@ -7521,7 +7521,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>9</v>
       </c>
@@ -7547,7 +7547,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="33" spans="2:10">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>10</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="34" spans="2:10">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>11</v>
       </c>
@@ -7602,7 +7602,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="2:10">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35">
         <f>SUM(C23:C34)</f>
         <v>1</v>
@@ -7640,24 +7640,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.5" style="4" customWidth="1"/>
-    <col min="5" max="6" width="12.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="22" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="22"/>
+    <col min="4" max="4" width="11.42578125" style="4" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="22" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -7734,7 +7734,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -7788,7 +7788,7 @@
         <v>0.745</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -7842,7 +7842,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11">
         <f>SUM(C3:C10)</f>
         <v>1</v>
@@ -7920,7 +7920,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -7935,7 +7935,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -7953,7 +7953,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>59</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>0.92999999999999994</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>3</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>0.94799999999999995</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>4</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>5</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>0.97799999999999998</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>6</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>7</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C25">
         <f>SUM(C17:C24)</f>
         <v>1</v>
@@ -8224,7 +8224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G26" s="22" t="s">
         <v>45</v>
       </c>
@@ -8246,24 +8246,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="22" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -8286,7 +8286,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>0.42000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -8364,7 +8364,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -8390,7 +8390,7 @@
         <v>0.58000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -8442,7 +8442,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -8468,7 +8468,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -8497,7 +8497,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11">
         <f>SUM(C3:C10)</f>
         <v>1</v>
@@ -8515,7 +8515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -8526,7 +8526,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -8550,7 +8550,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>59</v>
       </c>
@@ -8573,7 +8573,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0</v>
       </c>
@@ -8599,7 +8599,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>3</v>
       </c>
@@ -8677,7 +8677,7 @@
         <v>0.84499999999999997</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>4</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>0.93499999999999994</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>5</v>
       </c>
@@ -8729,7 +8729,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>6</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>7</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C25">
         <f>SUM(C17:C24)</f>
         <v>1</v>
@@ -8824,23 +8824,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="22"/>
-    <col min="9" max="9" width="8.83203125" style="22"/>
+    <col min="4" max="4" width="13.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="22"/>
+    <col min="9" max="9" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -8889,7 +8889,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>0.65999999999999992</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>0.80999999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>0.81699999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -8993,7 +8993,7 @@
         <v>0.91699999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>0.93699999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -9045,7 +9045,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -9074,7 +9074,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11">
         <f>SUM(C3:C10)</f>
         <v>1</v>
@@ -9092,7 +9092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -9116,12 +9116,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>59</v>
       </c>
@@ -9144,7 +9144,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0</v>
       </c>
@@ -9170,7 +9170,7 @@
         <v>0.68300000000000005</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1</v>
       </c>
@@ -9196,7 +9196,7 @@
         <v>0.79300000000000004</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2</v>
       </c>
@@ -9222,7 +9222,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>3</v>
       </c>
@@ -9248,7 +9248,7 @@
         <v>0.94000000000000006</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>4</v>
       </c>
@@ -9274,7 +9274,7 @@
         <v>0.97000000000000008</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>5</v>
       </c>
@@ -9300,7 +9300,7 @@
         <v>0.97400000000000009</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>6</v>
       </c>
@@ -9326,7 +9326,7 @@
         <v>0.9900000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>7</v>
       </c>
@@ -9352,7 +9352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>SUM(C18:C25)</f>
         <v>1</v>
@@ -9373,7 +9373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>45</v>
       </c>
@@ -9401,23 +9401,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="22"/>
+    <col min="4" max="4" width="13.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -9440,7 +9440,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -9466,7 +9466,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -9492,7 +9492,7 @@
         <v>0.22999999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -9518,7 +9518,7 @@
         <v>0.27999999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>0.62999999999999989</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>0.67999999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -9596,7 +9596,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -9622,7 +9622,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -9674,7 +9674,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -9700,7 +9700,7 @@
         <v>0.95000000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -9729,7 +9729,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14">
         <f>SUM(C3:C13)</f>
         <v>1</v>
@@ -9747,7 +9747,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -9758,7 +9758,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -9797,7 +9797,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0</v>
       </c>
@@ -9823,7 +9823,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>1</v>
       </c>
@@ -9849,7 +9849,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2</v>
       </c>
@@ -9875,7 +9875,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>3</v>
       </c>
@@ -9901,7 +9901,7 @@
         <v>0.87999999999999989</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>4</v>
       </c>
@@ -9927,7 +9927,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>5</v>
       </c>
@@ -9953,7 +9953,7 @@
         <v>0.91999999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>6</v>
       </c>
@@ -9979,7 +9979,7 @@
         <v>0.92999999999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>7</v>
       </c>
@@ -10005,7 +10005,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>8</v>
       </c>
@@ -10031,7 +10031,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>9</v>
       </c>
@@ -10060,7 +10060,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>10</v>
       </c>
@@ -10086,7 +10086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C30">
         <f>SUM(C19:C29)</f>
         <v>1</v>
@@ -10121,22 +10121,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="22"/>
+    <col min="4" max="4" width="11.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -10159,7 +10159,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -10211,7 +10211,7 @@
         <v>0.15000000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -10237,7 +10237,7 @@
         <v>0.18000000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -10263,7 +10263,7 @@
         <v>0.44000000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -10289,7 +10289,7 @@
         <v>0.47000000000000008</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -10315,7 +10315,7 @@
         <v>0.4900000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -10341,7 +10341,7 @@
         <v>0.53000000000000014</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -10367,7 +10367,7 @@
         <v>0.68000000000000016</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -10393,7 +10393,7 @@
         <v>0.7200000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -10419,7 +10419,7 @@
         <v>0.79000000000000026</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -10445,7 +10445,7 @@
         <v>0.89000000000000024</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
@@ -10471,7 +10471,7 @@
         <v>0.94000000000000028</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>12</v>
       </c>
@@ -10497,7 +10497,7 @@
         <v>0.98000000000000032</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
@@ -10526,7 +10526,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17">
         <f>SUM(C3:C16)</f>
         <v>1.0000000000000002</v>
@@ -10544,7 +10544,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -10552,7 +10552,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -10561,12 +10561,12 @@
         <v>5.6000000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>59</v>
       </c>
@@ -10589,7 +10589,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0</v>
       </c>
@@ -10615,7 +10615,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1</v>
       </c>
@@ -10641,7 +10641,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>2</v>
       </c>
@@ -10667,7 +10667,7 @@
         <v>0.43000000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>3</v>
       </c>
@@ -10693,7 +10693,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>4</v>
       </c>
@@ -10719,7 +10719,7 @@
         <v>0.71000000000000008</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>5</v>
       </c>
@@ -10745,7 +10745,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>6</v>
       </c>
@@ -10771,7 +10771,7 @@
         <v>0.82000000000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>7</v>
       </c>
@@ -10797,7 +10797,7 @@
         <v>0.87000000000000011</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>8</v>
       </c>
@@ -10823,7 +10823,7 @@
         <v>0.91000000000000014</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>9</v>
       </c>
@@ -10849,7 +10849,7 @@
         <v>0.93000000000000016</v>
       </c>
     </row>
-    <row r="33" spans="2:10">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>10</v>
       </c>
@@ -10875,7 +10875,7 @@
         <v>0.96000000000000019</v>
       </c>
     </row>
-    <row r="34" spans="2:10">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>11</v>
       </c>
@@ -10901,7 +10901,7 @@
         <v>0.9800000000000002</v>
       </c>
     </row>
-    <row r="35" spans="2:10">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>12</v>
       </c>
@@ -10927,7 +10927,7 @@
         <v>0.99000000000000021</v>
       </c>
     </row>
-    <row r="36" spans="2:10">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>13</v>
       </c>
@@ -10953,7 +10953,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="37" spans="2:10">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37">
         <f>SUM(C23:C36)</f>
         <v>1.0000000000000002</v>

</xml_diff>

<commit_message>
Rectified [12:16] to [11:15] in allBenchmarks.csv
</commit_message>
<xml_diff>
--- a/sanitized.xlsx
+++ b/sanitized.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="560" windowWidth="22560" windowHeight="13360" activeTab="10"/>
+    <workbookView xWindow="280" yWindow="600" windowWidth="22560" windowHeight="13360" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="impacts" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="97">
   <si>
     <t>astar</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>Trial2_1_old</t>
+  </si>
+  <si>
+    <t>Trial3</t>
   </si>
 </sst>
 </file>
@@ -2152,7 +2155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -4978,7 +4981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
@@ -9123,10 +9126,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9469,7 +9472,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>0</v>
       </c>
@@ -9496,7 +9499,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>1</v>
       </c>
@@ -9523,7 +9526,7 @@
         <v>0.83400000000000007</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>2</v>
       </c>
@@ -9550,7 +9553,7 @@
         <v>0.96400000000000008</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>3</v>
       </c>
@@ -9577,7 +9580,7 @@
         <v>0.97600000000000009</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>4</v>
       </c>
@@ -9607,7 +9610,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>5</v>
       </c>
@@ -9634,7 +9637,7 @@
         <v>0.9890000000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>6</v>
       </c>
@@ -9664,7 +9667,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>7</v>
       </c>
@@ -9691,7 +9694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C25">
         <f>SUM(C17:C24)</f>
         <v>1</v>
@@ -9709,9 +9712,281 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G26" s="22" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C27">
+        <f>0.7*8</f>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0.37</v>
+      </c>
+      <c r="D29" s="4">
+        <v>6500</v>
+      </c>
+      <c r="E29" s="8">
+        <f>C29*D29</f>
+        <v>2405</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="22">
+        <f>E29/$E$25</f>
+        <v>0.39487726787620064</v>
+      </c>
+      <c r="H29">
+        <v>0.39</v>
+      </c>
+      <c r="I29" s="35">
+        <f>C29</f>
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E30" s="8">
+        <f t="shared" ref="E30:E36" si="6">C30*D30</f>
+        <v>912</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="22">
+        <f t="shared" ref="G30:G36" si="7">E30/$E$25</f>
+        <v>0.14974140054182744</v>
+      </c>
+      <c r="H30">
+        <v>0.17</v>
+      </c>
+      <c r="I30" s="35">
+        <f>C30+I29</f>
+        <v>0.67399999999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>0.08</v>
+      </c>
+      <c r="D31" s="4">
+        <v>7500</v>
+      </c>
+      <c r="E31" s="8">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="22">
+        <f t="shared" si="7"/>
+        <v>9.8514079303833837E-2</v>
+      </c>
+      <c r="H31">
+        <v>0.11</v>
+      </c>
+      <c r="I31" s="35">
+        <f t="shared" ref="I31:I36" si="8">C31+I30</f>
+        <v>0.75399999999999989</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>0.12</v>
+      </c>
+      <c r="D32" s="4">
+        <v>5000</v>
+      </c>
+      <c r="E32" s="8">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="22">
+        <f t="shared" si="7"/>
+        <v>9.8514079303833837E-2</v>
+      </c>
+      <c r="H32">
+        <v>0.1</v>
+      </c>
+      <c r="I32" s="35">
+        <f t="shared" si="8"/>
+        <v>0.87399999999999989</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>0.05</v>
+      </c>
+      <c r="D33" s="4">
+        <v>10900</v>
+      </c>
+      <c r="E33" s="8">
+        <f t="shared" si="6"/>
+        <v>545</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="22">
+        <f t="shared" si="7"/>
+        <v>8.9483622034315743E-2</v>
+      </c>
+      <c r="H33">
+        <v>0.09</v>
+      </c>
+      <c r="I33" s="35">
+        <f t="shared" si="8"/>
+        <v>0.92399999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>0.06</v>
+      </c>
+      <c r="D34" s="4">
+        <v>8000</v>
+      </c>
+      <c r="E34" s="8">
+        <f t="shared" si="6"/>
+        <v>480</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="22">
+        <f t="shared" si="7"/>
+        <v>7.8811263443067076E-2</v>
+      </c>
+      <c r="H34">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I34" s="35">
+        <f t="shared" si="8"/>
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D35" s="4">
+        <v>26500</v>
+      </c>
+      <c r="E35" s="8">
+        <f t="shared" si="6"/>
+        <v>397.5</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="22">
+        <f t="shared" si="7"/>
+        <v>6.5265577538789921E-2</v>
+      </c>
+      <c r="H35">
+        <v>0.06</v>
+      </c>
+      <c r="I35" s="35">
+        <f t="shared" si="8"/>
+        <v>0.999</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>1E-3</v>
+      </c>
+      <c r="D36" s="4">
+        <v>37500</v>
+      </c>
+      <c r="E36" s="8">
+        <f t="shared" si="6"/>
+        <v>37.5</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="22">
+        <f t="shared" si="7"/>
+        <v>6.1571299564896148E-3</v>
+      </c>
+      <c r="H36">
+        <v>0.01</v>
+      </c>
+      <c r="I36" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <f>SUM(C29:C36)</f>
+        <v>1</v>
+      </c>
+      <c r="E37" s="8">
+        <f>SUM(E29:E36)</f>
+        <v>5977</v>
+      </c>
+      <c r="G37" s="22">
+        <f>SUM(G29:G36)</f>
+        <v>0.98136441999835811</v>
+      </c>
+      <c r="H37">
+        <f>SUM(H29:H36)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>